<commit_message>
Update BOM for Capstone Review
</commit_message>
<xml_diff>
--- a/Hardware/Documentation/BOM/GeneralPurposeAlarmDevicePCB-Capstone2023WifiBatt.xlsx
+++ b/Hardware/Documentation/BOM/GeneralPurposeAlarmDevicePCB-Capstone2023WifiBatt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trent\Documents\GitHub\TF-general-alarm-device\Hardware\Documentation\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAEFAAB-1F6D-4AE2-90FF-5DF4D1067DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A40B6C-C92C-4237-A444-D8E221516FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="156">
   <si>
     <t>Reference</t>
   </si>
@@ -480,12 +480,39 @@
   </si>
   <si>
     <t>Aokin ESP32 ESP-WROOM-32</t>
+  </si>
+  <si>
+    <t>Parts for Implementation for one device</t>
+  </si>
+  <si>
+    <t>Total Cost:</t>
+  </si>
+  <si>
+    <t>Semester Parts Cost</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>USB Li-ion Charger</t>
+  </si>
+  <si>
+    <t>3.7V 2500mAh LiPo Battery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -495,12 +522,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -515,8 +548,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,6 +571,38 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90B302D5-1EF0-4597-861D-1CB5E36C9ED6}" name="Table2" displayName="Table2" ref="A3:W17" totalsRowShown="0">
+  <autoFilter ref="A3:W17" xr:uid="{90B302D5-1EF0-4597-861D-1CB5E36C9ED6}"/>
+  <tableColumns count="23">
+    <tableColumn id="1" xr3:uid="{C70581A4-DCE4-48A8-B231-1BEE3D01EE7E}" name="Reference"/>
+    <tableColumn id="2" xr3:uid="{9FEC1424-2376-4A06-9E8E-353ACA0CE243}" name="Value"/>
+    <tableColumn id="3" xr3:uid="{1D97125B-E401-4A7D-B2DC-90A41696BE32}" name="Footprint"/>
+    <tableColumn id="4" xr3:uid="{3FBD4B81-433B-4E42-8720-EB49A04C5A18}" name="Datasheet"/>
+    <tableColumn id="5" xr3:uid="{1E81605A-0160-44C3-9400-D8C0E0B1612E}" name="Assembly Type"/>
+    <tableColumn id="6" xr3:uid="{B299A0DA-58F1-4925-B37B-BD8EC19953BC}" name="AssemblyType"/>
+    <tableColumn id="7" xr3:uid="{0585B61D-7A8F-4086-BDB9-2B3A46B1EAF8}" name="Category"/>
+    <tableColumn id="8" xr3:uid="{91BEFA00-272E-4A26-8AB5-1AC2F1850C6A}" name="Cost"/>
+    <tableColumn id="9" xr3:uid="{24E364B6-528E-47EF-A7B2-C906542F706B}" name="DK_Datasheet_Link"/>
+    <tableColumn id="10" xr3:uid="{9BF76540-2F1C-4064-A2DC-D6A9DDBA4C9F}" name="DK_Detail_Page"/>
+    <tableColumn id="11" xr3:uid="{756CB9CE-2BE2-4FDE-A869-2C604B1936FE}" name="Description"/>
+    <tableColumn id="12" xr3:uid="{8E28BC8B-6A51-4623-B7E9-6F1FCCC4A101}" name="Digi-Key_PN"/>
+    <tableColumn id="13" xr3:uid="{81AC27C9-7DF2-4A2F-8D81-B0F1CB29B491}" name="Distributor 1"/>
+    <tableColumn id="14" xr3:uid="{88734597-FC7E-4A6D-8BE3-308645C010FB}" name="Distributor 1 PN"/>
+    <tableColumn id="15" xr3:uid="{F3CA7586-DEDF-4D48-B4C6-F4DCEB0B21C5}" name="Distributor 2"/>
+    <tableColumn id="16" xr3:uid="{E45B6735-CF36-4C06-AD37-0DBA1C8B9AE6}" name="Distributor 2 PN"/>
+    <tableColumn id="17" xr3:uid="{A8E495EA-898E-4B84-BE76-9262C724EC90}" name="Family"/>
+    <tableColumn id="18" xr3:uid="{CFF1A355-2DCA-4C03-8F57-8CF6167812F7}" name="MPN"/>
+    <tableColumn id="19" xr3:uid="{B9F7740B-CC8C-4B9F-A04B-AD304C010541}" name="MPN "/>
+    <tableColumn id="20" xr3:uid="{E63E5F61-16A4-4A0C-A423-43CC2C830497}" name="Manufacturer"/>
+    <tableColumn id="21" xr3:uid="{8C59AF21-4689-4801-B53F-0DFB4BB70EB5}" name="Manufacturer "/>
+    <tableColumn id="22" xr3:uid="{417AFDCA-C7D9-48B3-8819-936DF4594212}" name="Status"/>
+    <tableColumn id="23" xr3:uid="{096F45CD-EF54-4102-B090-0067BB00A9FC}" name="Qty"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -797,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W66"/>
+  <dimension ref="A2:W66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,164 +879,111 @@
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="17.21875" customWidth="1"/>
     <col min="3" max="3" width="27.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="51.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="6.77734375" customWidth="1"/>
+    <col min="11" max="11" width="40.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" customWidth="1"/>
+    <col min="16" max="16" width="8.21875" customWidth="1"/>
+    <col min="20" max="20" width="11.109375" customWidth="1"/>
+    <col min="21" max="21" width="3.33203125" customWidth="1"/>
+    <col min="22" max="22" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2">
-        <v>12.99</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
+      <c r="A2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3">
-        <v>6.8000000000000005E-4</v>
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
       </c>
       <c r="M3" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="N3" t="s">
-        <v>38</v>
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>16</v>
       </c>
       <c r="R3" t="s">
-        <v>39</v>
+        <v>17</v>
+      </c>
+      <c r="S3" t="s">
+        <v>18</v>
       </c>
       <c r="T3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="U3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -973,41 +991,20 @@
       <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
       <c r="H4">
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" t="s">
-        <v>45</v>
+        <v>12.99</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" t="s">
-        <v>48</v>
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>30</v>
       </c>
       <c r="Q4" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" t="s">
-        <v>50</v>
-      </c>
-      <c r="T4" t="s">
-        <v>51</v>
-      </c>
-      <c r="V4" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="W4">
         <v>1</v>
@@ -1015,55 +1012,37 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
       <c r="H5">
-        <v>2.1499999999999998E-2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" t="s">
-        <v>58</v>
+        <v>6.8000000000000005E-4</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
-      </c>
-      <c r="L5" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="M5" t="s">
         <v>34</v>
       </c>
       <c r="N5" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="R5" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="T5" t="s">
-        <v>51</v>
-      </c>
-      <c r="V5" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="W5">
         <v>1</v>
@@ -1071,90 +1050,111 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
         <v>43</v>
       </c>
       <c r="H6">
-        <v>3.7499999999999999E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="M6" t="s">
         <v>34</v>
       </c>
       <c r="N6" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="Q6" t="s">
         <v>49</v>
       </c>
       <c r="R6" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="T6" t="s">
         <v>51</v>
       </c>
+      <c r="V6" t="s">
+        <v>52</v>
+      </c>
       <c r="W6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
       </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
       <c r="H7">
-        <v>0.48</v>
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" t="s">
+        <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>75</v>
+        <v>59</v>
+      </c>
+      <c r="L7" t="s">
+        <v>60</v>
       </c>
       <c r="M7" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="N7" t="s">
-        <v>77</v>
+        <v>61</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>49</v>
       </c>
       <c r="R7" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="T7" t="s">
-        <v>79</v>
+        <v>51</v>
+      </c>
+      <c r="V7" t="s">
+        <v>52</v>
       </c>
       <c r="W7">
         <v>1</v>
@@ -1162,55 +1162,52 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="H8">
-        <v>0.17</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="I8" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="K8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="L8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="M8" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="N8" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="Q8" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="R8" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="T8" t="s">
-        <v>81</v>
-      </c>
-      <c r="V8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="W8">
         <v>1</v>
@@ -1218,55 +1215,37 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="F9" t="s">
         <v>33</v>
       </c>
-      <c r="G9" t="s">
-        <v>91</v>
-      </c>
       <c r="H9">
-        <v>0.46</v>
-      </c>
-      <c r="I9" t="s">
-        <v>95</v>
-      </c>
-      <c r="J9" t="s">
-        <v>96</v>
+        <v>0.48</v>
       </c>
       <c r="K9" t="s">
-        <v>97</v>
-      </c>
-      <c r="L9" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="M9" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="N9" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="R9" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="T9" t="s">
-        <v>100</v>
-      </c>
-      <c r="V9" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="W9">
         <v>1</v>
@@ -1274,37 +1253,55 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>86</v>
       </c>
       <c r="H10">
-        <v>1.5E-3</v>
+        <v>0.17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10" t="s">
+        <v>87</v>
       </c>
       <c r="K10" t="s">
-        <v>104</v>
+        <v>88</v>
+      </c>
+      <c r="L10" t="s">
+        <v>89</v>
       </c>
       <c r="M10" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="N10" t="s">
-        <v>105</v>
+        <v>89</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>80</v>
       </c>
       <c r="R10" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="T10" t="s">
-        <v>102</v>
+        <v>81</v>
+      </c>
+      <c r="V10" t="s">
+        <v>52</v>
       </c>
       <c r="W10">
         <v>1</v>
@@ -1312,48 +1309,66 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
       </c>
+      <c r="G11" t="s">
+        <v>91</v>
+      </c>
       <c r="H11">
-        <v>1.5E-3</v>
+        <v>0.46</v>
+      </c>
+      <c r="I11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" t="s">
+        <v>96</v>
       </c>
       <c r="K11" t="s">
-        <v>108</v>
+        <v>97</v>
+      </c>
+      <c r="L11" t="s">
+        <v>98</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="N11" t="s">
-        <v>109</v>
+        <v>98</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>99</v>
       </c>
       <c r="R11" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="T11" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="V11" t="s">
+        <v>52</v>
       </c>
       <c r="W11">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
         <v>101</v>
@@ -1365,19 +1380,19 @@
         <v>33</v>
       </c>
       <c r="H12">
-        <v>2.2000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="K12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="M12" t="s">
         <v>34</v>
       </c>
       <c r="N12" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="R12" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="T12" t="s">
         <v>102</v>
@@ -1388,10 +1403,10 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
         <v>101</v>
@@ -1403,33 +1418,33 @@
         <v>33</v>
       </c>
       <c r="H13">
-        <v>2.7000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="K13" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="M13" t="s">
         <v>34</v>
       </c>
       <c r="N13" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="R13" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="T13" t="s">
         <v>102</v>
       </c>
       <c r="W13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
         <v>101</v>
@@ -1440,26 +1455,23 @@
       <c r="F14" t="s">
         <v>33</v>
       </c>
-      <c r="G14" t="s">
-        <v>123</v>
-      </c>
       <c r="H14">
-        <v>2.29E-2</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="K14" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="M14" t="s">
         <v>34</v>
       </c>
       <c r="N14" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="R14" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="T14" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="W14">
         <v>1</v>
@@ -1467,37 +1479,199 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>101</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>146</v>
+        <v>33</v>
       </c>
       <c r="H15">
-        <v>8.99</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="K15" t="s">
-        <v>145</v>
-      </c>
-      <c r="O15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P15" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>140</v>
+        <v>118</v>
+      </c>
+      <c r="M15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" t="s">
+        <v>119</v>
+      </c>
+      <c r="R15" t="s">
+        <v>120</v>
       </c>
       <c r="T15" t="s">
-        <v>141</v>
+        <v>102</v>
       </c>
       <c r="W15">
         <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16">
+        <v>2.29E-2</v>
+      </c>
+      <c r="K16" t="s">
+        <v>124</v>
+      </c>
+      <c r="M16" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" t="s">
+        <v>125</v>
+      </c>
+      <c r="R16" t="s">
+        <v>126</v>
+      </c>
+      <c r="T16" t="s">
+        <v>127</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>146</v>
+      </c>
+      <c r="H17">
+        <v>8.99</v>
+      </c>
+      <c r="K17" t="s">
+        <v>145</v>
+      </c>
+      <c r="O17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P17" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>140</v>
+      </c>
+      <c r="T17" t="s">
+        <v>141</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="2">
+        <v>23.19</v>
+      </c>
+      <c r="H19">
+        <f>SUM(Table2[Cost])</f>
+        <v>23.185880000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="2">
+        <v>93.94</v>
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.3">
@@ -1551,7 +1725,14 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A22:C22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>